<commit_message>
Add : StageDB 추가 및 StageDB CSV 로드 기능 구현
</commit_message>
<xml_diff>
--- a/Assets/Resources/AllDataBase.xlsx
+++ b/Assets/Resources/AllDataBase.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AB5CFD-B03E-480E-AA20-A96A48C83F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3465F8BB-781E-4699-9699-95F1774AF46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6FBF613A-6FA1-455C-A588-99C38EF2F98A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6FBF613A-6FA1-455C-A588-99C38EF2F98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="3" r:id="rId1"/>
     <sheet name="ItemDB" sheetId="2" r:id="rId2"/>
     <sheet name="EnemyDB" sheetId="4" r:id="rId3"/>
+    <sheet name="StageDB" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="85">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -341,6 +342,42 @@
   </si>
   <si>
     <t>MoveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChapterNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StageNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurStageModifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stageName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlayEnemyCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SummonEnemyIDList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처음의 숲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미숙한자들의 길</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>익숙해지는 주변</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,11 +424,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1435,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84F1D1A-9464-4F09-91F9-B0D7B5654210}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1877,4 +1917,143 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21794CA0-3139-48DB-BBB8-A2114802E57F}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>7000</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2">
+        <v>100101102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7001</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2">
+        <v>100101102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>7002</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5" s="2">
+        <v>102103104</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update : DataManager에 SellItemDB 추가
</commit_message>
<xml_diff>
--- a/Assets/Resources/AllDataBase.xlsx
+++ b/Assets/Resources/AllDataBase.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3465F8BB-781E-4699-9699-95F1774AF46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B14FA1-BB73-4251-B71A-4C4430A28E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6FBF613A-6FA1-455C-A588-99C38EF2F98A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6FBF613A-6FA1-455C-A588-99C38EF2F98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="3" r:id="rId1"/>
-    <sheet name="ItemDB" sheetId="2" r:id="rId2"/>
-    <sheet name="EnemyDB" sheetId="4" r:id="rId3"/>
-    <sheet name="StageDB" sheetId="5" r:id="rId4"/>
+    <sheet name="EnemyDB" sheetId="4" r:id="rId2"/>
+    <sheet name="StageDB" sheetId="5" r:id="rId3"/>
+    <sheet name="ItemDB" sheetId="2" r:id="rId4"/>
+    <sheet name="SellItemDB" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="104">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -378,6 +379,81 @@
   </si>
   <si>
     <t>익숙해지는 주변</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OriginID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProductID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1002,1003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1002,1004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1002,2003,2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1002,2003,2001</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실버,골드검세트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황동,골드검세트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검+회복포션세트1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검+회복포션세트2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복포션세트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전설의 회복포션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StackCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsStack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PriceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diamond</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -424,7 +500,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -432,6 +508,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -820,11 +899,598 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84F1D1A-9464-4F09-91F9-B0D7B5654210}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="3" max="3" width="39.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5">
+        <v>200</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>250</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>0.8</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7">
+        <v>300</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>0.8</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5005</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>350</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.8</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5006</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1.2</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5007</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1.2</v>
+      </c>
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5008</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1.2</v>
+      </c>
+      <c r="J11">
+        <v>30</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21794CA0-3139-48DB-BBB8-A2114802E57F}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>7000</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2">
+        <v>100101102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7001</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2">
+        <v>100101102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>7002</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5" s="2">
+        <v>102103104</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B71D793-0238-48D3-9657-8754CE8C134C}">
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1471,493 +2137,44 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84F1D1A-9464-4F09-91F9-B0D7B5654210}">
-  <dimension ref="A1:L11"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9170D880-A928-4262-B4C1-2F8BC23700B7}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
-    <col min="3" max="3" width="39.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.75" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>5000</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>5001</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4">
-        <v>150</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>5002</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5">
-        <v>200</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5003</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6">
-        <v>250</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>0.8</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5004</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7">
-        <v>300</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>0.8</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>5</v>
-      </c>
-      <c r="L7">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>5005</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8">
-        <v>350</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0.8</v>
-      </c>
-      <c r="J8">
-        <v>30</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5006</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9">
-        <v>50</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1.2</v>
-      </c>
-      <c r="J9">
-        <v>50</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>5007</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10">
-        <v>50</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1.2</v>
-      </c>
-      <c r="J10">
-        <v>100</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>5008</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11">
-        <v>50</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>1.2</v>
-      </c>
-      <c r="J11">
-        <v>30</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21794CA0-3139-48DB-BBB8-A2114802E57F}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.75" customWidth="1"/>
+    <col min="6" max="7" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1965,91 +2182,229 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3" s="2">
-        <v>100101102</v>
+        <v>1000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>7001</v>
+        <v>10001</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
-      <c r="G4" s="2">
-        <v>100101102</v>
+        <v>1001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4">
+        <v>1100</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>7002</v>
+        <v>10002</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
+        <v>1002</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5">
+        <v>1200</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10003</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6">
+        <v>1300</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10004</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7">
+        <v>1400</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10005</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8">
+        <v>1500</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>10006</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9">
+        <v>1600</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10007</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10">
+        <v>1700</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5" s="2">
-        <v>102103104</v>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10008</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2003</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11">
+        <v>1800</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>